<commit_message>
started finalising the documents
</commit_message>
<xml_diff>
--- a/Testing/Testdokumente/Old/Fehlersammlung/Fehlersammlung V 2.xlsx
+++ b/Testing/Testdokumente/Old/Fehlersammlung/Fehlersammlung V 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmenschmider/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josua_duyp43m\Documents\Documentation\Testing\Testdokumente\Old\Fehlersammlung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2325F3DD-94A0-9A45-9BB2-FBE0BDB67536}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E0B1196-D314-4F74-91E5-15E4387E9A2E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25980" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25980" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -58,12 +58,6 @@
     <t>1,1/1,2</t>
   </si>
   <si>
-    <t>Login Wahlleiter/ Moderator/ Admin</t>
-  </si>
-  <si>
-    <t>Login Moderator, Wahlleiter, Admin</t>
-  </si>
-  <si>
     <t>Anastasia</t>
   </si>
   <si>
@@ -125,6 +119,12 @@
   </si>
   <si>
     <t>V2</t>
+  </si>
+  <si>
+    <t>Login Moderator, Wahlleiter</t>
+  </si>
+  <si>
+    <t>Login Wahlleiter/ Moderator</t>
   </si>
 </sst>
 </file>
@@ -322,6 +322,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -338,12 +344,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1509,31 +1509,31 @@
   <dimension ref="A1:IV10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
-    <col min="2" max="3" width="15.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
-    <col min="5" max="11" width="11.5" style="1" customWidth="1"/>
-    <col min="12" max="256" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" customWidth="1"/>
+    <col min="5" max="11" width="11.42578125" style="1" customWidth="1"/>
+    <col min="12" max="256" width="10.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="20"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3" t="s">
         <v>3</v>
@@ -1548,7 +1548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1579,24 +1579,24 @@
       </c>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C3" s="8">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E3" s="9">
         <v>1.2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="5" t="s">
@@ -1606,88 +1606,88 @@
         <v>43152</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>1.5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="9">
         <v>1.4</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>1.8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="8">
         <v>47</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="2"/>
       <c r="H5" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I5" s="10">
         <v>43211</v>
       </c>
       <c r="J5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="E6" s="9">
         <v>2.4</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="7"/>
@@ -1695,54 +1695,54 @@
       <c r="J6" s="7"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="2"/>
       <c r="H7" s="14"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="17"/>
     </row>
-    <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>13.1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="8">
         <v>45</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="2"/>
       <c r="H8" s="15"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>13.2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -1754,7 +1754,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>

</xml_diff>